<commit_message>
Got both google scrapping and line break to work
</commit_message>
<xml_diff>
--- a/data/review_data.xlsx
+++ b/data/review_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5688"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15192" windowHeight="5688"/>
   </bookViews>
   <sheets>
     <sheet name="review_data" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="114">
   <si>
     <t>Article name</t>
   </si>
@@ -62,11 +62,6 @@
     <t>My review</t>
   </si>
   <si>
-    <t>Overall decent article. Drawbacks are: 
-Missing details about sampling
-The 0-1 classifier may fail on real data set where failures are rare when trained on this data</t>
-  </si>
-  <si>
     <t>Data mining method for listed companies’ financial distress prediction</t>
   </si>
   <si>
@@ -74,11 +69,6 @@
   </si>
   <si>
     <t>DT</t>
-  </si>
-  <si>
-    <t>A lot of details are missing. It is not clear to me what the different tree/forest models are
-Very small sample with 35 covaraites
-Hard to say anything good about their sampling</t>
   </si>
   <si>
     <t>Random sampling with some sort of prior weight depending on covaraites. Details are not clear
@@ -113,23 +103,371 @@
     <t>Up to  95.9% AUC with cross validation</t>
   </si>
   <si>
-    <t>Credit for:
+    <t>DT, B, AdaBoost</t>
+  </si>
+  <si>
+    <t>Chinece firms from China
+Stock Market and Accounting Research Database
+Default indicator is 'specially treated (ST) by China Securities Supervision and Management Committee'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paired firms between 2000 and 2005
+Mix years / ignores longitudinal aspect
+Details about parring is not clear
+In addition they: '... eliminate outliers, companies with financial ratios deviating from the mean value as much as three times of standard deviation are excluded'
+</t>
+  </si>
+  <si>
+    <t>Introduces AdaBoost and shows how it can ba applied
+Compare with Neural Networks. I have too little knowledge about Neural Networks to judge their modeling
+Missing details about sampling
+The 0-1 classifier may fail on real data set where failures are rare when trained on this data</t>
+  </si>
+  <si>
+    <t>Bankruptcy prediction using support vector machine with optimal choice of kernel function parameters</t>
+  </si>
+  <si>
+    <t>Expert Systems with Applications</t>
+  </si>
+  <si>
+    <t>SVM, LOGI, NN, LDA</t>
+  </si>
+  <si>
+    <t>Data is from 'Korea’s largest credit guarantee organization' with 'all of the non-bankruptcy cases are from medium-sized heavy industry firms in 2002 and the corresponding bankruptcy cases are also from the same industry. In general, however, the number of bankruptcy cases is smaller than that of non-bankruptcy cases; hence, we collected additional bankruptcy cases from the years of 2000, 2001, and 2002'</t>
+  </si>
+  <si>
+    <t>All bankeruptcies and 944 random non-bankerupcies</t>
+  </si>
+  <si>
+    <t>944 / 944 (firms)</t>
+  </si>
+  <si>
+    <t>83% accuracy with hold-out (though C-cost and kernal parameter is trained on the whole data)</t>
+  </si>
+  <si>
+    <t>A Combination Use of Bagging and Random Subspace with Memory Mechanism for Dynamic Financial Distress Prediction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industrial Engineering and Engineering Management </t>
+  </si>
+  <si>
+    <t>NN, B</t>
+  </si>
+  <si>
+    <t>Does some sort of random forest, bagging with decision trees amd/or descision tree. It is not clear to me
+A lot of details are missing. It is not clear to me what the different tree/forest models are
+Very small sample with 35 covaraites
+Hard to say anything good about their sampling</t>
+  </si>
+  <si>
+    <t>Applies Extreme Gradient Boosting as the first as far as I am aware in this context. Further, they construct features with a quite simple method that do seem to work 
+Credit for:
 Large data set
 Interesting idea of synthetic features and Extreme Gradient Boosting
 Making the data set avilable (see http://bit.ly/2id2zk8)
 I am not sure how exactly the sampling is done
 Sad that the longitudinal aspect is ignored
-Little emphasis have been put on the other models they compare with. I have gotten +80% cross validation AUC with both Logit models and SVM with one days work</t>
-  </si>
-  <si>
-    <t>DT, B, AdaBoost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paired firms between 2000 and 2005
-Mix years / ignores longitudinal aspect
-Details about parring is not clear
-'In order to eliminate outliers, companies with financial ratios deviating from the mean value as much as three times of standard deviation are excluded'
+Little emphasis have been put on the other models they compare with. I have gotten +80% cross validation AUC with both Logit models and SVM with one days work with the data set</t>
+  </si>
+  <si>
+    <t>The main focus of the article is to use support vector machines in this context
+Credit for: 
+Comparing different kernals function
+Being one of the first to apply support vector machines is this context?
+Nice introduction of support vector machines using the standard library libsvm
+Nice illustration of SVM in 2D with principle components
+Sad that the longitudinal aspect is ignored
+Not directly applicable to real life data with the 50%-50% sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'Chinese listed companies is collected from CCER Economic and Financial Database'
+Defaults are defined as those where 'China Securities Supervision and Management
+Committee (CSSMC) carried out a 'Special Treatment (ST)' to warn the listed companies with negative net' profits in consecutive 2 years
+Uses financial data from firms 3 years prior with 'ST'
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All bankeruptcies in 2001-14
+Pair with non-bankrupt firms from the same industry, similar total assets and who do not have a 'ST' in the next 5 years </t>
+  </si>
+  <si>
+    <t>Up to 122 financial statements in one year. I gather it must be 50-50 split due to the pair sample</t>
+  </si>
+  <si>
+    <t>At best 80% accuracy (in-sample?)</t>
+  </si>
+  <si>
+    <t>They compare different ways of accountning for time-varying effects with neural networks. In essence, they use data in slidding window for their best model. Further, they apply an ensamble method where variables in each fit is random 
+It is nice that they account for the longitudinal aspect of data 
+Getting at best 80% accuracy (in-sample?) with a small data set with neural networks and 36 variables seems too low when further considering that we are looking at listed firms. Hence, data should be rather "clean"/homogeneous
+Paired sample</t>
+  </si>
+  <si>
+    <t>Additive Intensity Regression Models in Corporate Default Analysis</t>
+  </si>
+  <si>
+    <t>JOURNAL OF FINANCIAL ECONOMETRICS</t>
+  </si>
+  <si>
+    <t>AH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">370 / 2557 firms with multiple financial statements from each firm </t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Uses additive intensity (Aalen) models from the timereg package in R. The study is descriptive and shows that the coeffecient in typical models used (e.g. Shumway (2001)) in default prediction may be time-varying. The model baseline hazard with macro economic variables
+Cons:
+Descriptive study that cannot be used for prediction</t>
+  </si>
+  <si>
+    <t>Forecasting Bankruptcy More Accurately: A Simple Hazard Model</t>
+  </si>
+  <si>
+    <t>The Journal of Business</t>
+  </si>
+  <si>
+    <t>LOGI</t>
+  </si>
+  <si>
+    <t>US listed firms with Default indicators from  Moody’s Default Risk Service Database with financial data from  CRSP (Center for Research in Security Prices)
+Excludes 'All consecutive default events occurring within a 1-month horizon of any previously registered default ascribed to the same parent company' and financial firms
+Use data from  January 1, 1982 to January 1, 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US listed firms with accounting data from  Compustat Industrial File and the CRSP Daily Stock Return File. Defaults data 'from the Wall Street Journal Index, the Capital Changes Reporter, and the Compustat Research File. I also searched for firms whose stock was delisted from the NYSE or AMEX in the Directory of Obsolete Securities (Financial Stock Guide Service [1993]) and Nexis. All firms that filed for any type of bankruptcy within 5 years of delisting are considered bankrupt'
+Include firms that began trading before 1962 or after 1992 and financial firms are excluded </t>
+  </si>
+  <si>
+    <t>At most 33621 financial statements and 291 bankruptcies</t>
+  </si>
+  <si>
+    <t>Report decile ranking for out-sample-test (in time) that are hard to summarize in a table cell</t>
+  </si>
+  <si>
+    <t>A Comparison of Corporate Bankruptcy Models in Australia: The Merton vs. Accounting-based Models</t>
+  </si>
+  <si>
+    <t>'Companies listed on the Australian Stock Exchange (ASX) during 1990-2003. Bankruptcy data is collected from two sources: The website of www.delisted.com.au and Delisted Companies (1900-2003) by Financial Analysis Publications'
+The default indicator is in 'the strict legal sense' of administration, receivership, or liquidation
+Covariates are from Aspect Fin Analysis and/or Aspect Dat Analysis and Thomson Financial Datastream
+Financial firms are excluded</t>
+  </si>
+  <si>
+    <t>Showed how to fit a variable with logistic regression where one takes the longitudinal aspect of each firm into account. Further, illustrates how not doing this can imply bias with a small example thus implying a huge crituque of previous studies. Compares a model with previous used models. Lags accounting variables. Lastly, one of the first to the best of my knowledge who does out-sample test by using data from the following year 
+Changed the literature and is one prime papers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">93 / 1144 firms with multiple financial statements from each firm </t>
+  </si>
+  <si>
+    <t>Report expected cost measure of classification errors (ECM) with an cut-off value to get 0-1 variable with different cost values. Also reports deciles like Shumway (2001)</t>
+  </si>
+  <si>
+    <t>Compares the variables from Altman (1968), Zmijewski (1984), and Shumway (2001) in logic model with the Merton model. Further, they make a combination and find the best performance
+Nice with a study for Australian. Interesting that they find that the Merton model out-performs the other
+It is unclear to me whether the reported Forecasting Accuracy is in-sample or out-sample</t>
+  </si>
+  <si>
+    <t>'approximately 300,000 annual accounts of which almost 8,000 from failed companies'</t>
+  </si>
+  <si>
+    <t>'Danish public limited liability companies (A/S) and private limited liability companies (ApS)' with accounting data from KOB A/S 
+Estimation sample covers the period 1995-99
+Default is defined as:
+'The company is being liquidated or is subject to compulsory liquidation
+The company has been dissolved, dissolved by the courts, or is subject to compulsory dissolution by the court
+The company is subject to a compulsory deed of arrangement with creditors or is subject to a compulsory scheme of arrangement with creditors'
+Holding companies consolidated accounts and company with less than 50000 DKK is excluded</t>
+  </si>
+  <si>
+    <t>(In sample?) AUC of 82.5</t>
+  </si>
+  <si>
+    <t>Uses logistic regresion with a few new / non-commenly used covaraites
+Use a large sample of firms
+Finds that: 
+Critical auditor comment is quite significant
+Some differences with a sector by sector model
+Firms size (in terms of number of employees) have impact on the ability to predict in sample and on estimates</t>
+  </si>
+  <si>
+    <t>Modelling The Credit Risk Of The Hungarian Sme Sector</t>
+  </si>
+  <si>
+    <t>mnb</t>
+  </si>
+  <si>
+    <t>Up to 2629468 financial statements and 173664 firms</t>
+  </si>
+  <si>
+    <t>Hungarian firms with financial statements which was submitted to the Hungarian Natonal Tax and Customs Administraton
+Default data is from Central Credit Informaton System (KHR) which gather informaton about all loan and loan-type contracts
+'... government- or local government-owned companies (above a 25 per cent ownership rato), non-proft insttutons serving households and fnancial corporatons were fltered out'
+Default is defined as '[the firm] were in default with at least 10 per cent of their contracts' within a year where a contract is considered to have defaulted if '30-day defaults [are] ongoing for at least 60 days' 
+Data from 2007 to 2014</t>
+  </si>
+  <si>
+    <t>Out sample (in time) AUCs between 69%-81%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model firm failure for micro, small and medium-sized enterprises with logistic models
+Categorize firms in terms of sales figures and employees
+Use macro economics variables
+As rightly mentioned, the banks may introduce a selection bias with which firms that are in the sample
+May provide evidence that larger firms are more homogeneous and their credit risk depends more on the fnancial indicators of
+the company
+Cons:
+Including a dummy variable for all the years from age 1, 2, 3, ..., 24 a category for +25 seems alarming to me
+The continuous dropping of variable (including age factor levels) based on arguments like: '... we did not include the liquidity positon of microenterprises, since we are not convinced that greater liquidity would directly increase the credit risk of a company'
+Comparing estimates signs and magnitudes with different specification of the linear predictor due to the previous comment
+</t>
+  </si>
+  <si>
+    <t>Prediction of Financial Distress Companies on Bursa Malaysia Using Adaptive Neuro-Fuzzy Inference System</t>
+  </si>
+  <si>
+    <t>SMR</t>
+  </si>
+  <si>
+    <t>A Failure-Rate Model for the Danish Corporate Sector</t>
+  </si>
+  <si>
+    <t>Asia-Pacific Journal of Risk and Insurance</t>
+  </si>
+  <si>
+    <t>Probability-of-default curve calibration and the validation of internal rating systems</t>
+  </si>
+  <si>
+    <t>298 / 5091 financial statements</t>
+  </si>
+  <si>
+    <t>Approach to the assessment of credit risk for non-financial corporations. Poland Evidence</t>
+  </si>
+  <si>
+    <t>See 'Probability-of-default curve calibration and the validation of internal rating systems'</t>
+  </si>
+  <si>
+    <t>See 'Probability-of-default curve calibration and the validation of internal rating systems'
+I only quickly scanned this but what I saw did not seem resonable / worth reading</t>
+  </si>
+  <si>
+    <t>None?</t>
+  </si>
+  <si>
+    <t>accuracy rate of 86% though it is not clear to me whether this is in or out sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While the Adaptive Neuro-Fuzzy Inference System may be useful getting 86% on a small data set with a parsimonious model relative to the sample size is not convincing to me
+I gather some sort of sampling must have been done since ‘PN17 stands for Practice Note 17/2005 and is issued by Bursa Malaysia; relating to companies that are in financial distress’ (web source)
+</t>
+  </si>
+  <si>
+    <t>'distressed and nondistressed companies were collected for five years prior tobeing listed under the PN17 categories by the Bursa Malaysia. For example, for a company which was announced as distressed in 2015, the variables were computed for the year 2014 (year 1), 2013 (year 2), 2012 (year 3), 2010 (year 4) and2009 (year 5). The name of companies listed under PN17 was obtained from the Media Releases and Companies Announcements from the Bursa Malaysia website, while thefinancial data were collected from the Thomson Reuters Datastream'</t>
+  </si>
+  <si>
+    <t>20 / 44 where there is a 50%-50% split to in training</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polish firms from 2007 to 2012
+Defaults from Narodowy Bank Polski and National Court Register (KRS)
+Financial data from AMADEUS (Bureau van Dijk); Notoria OnLine
+Some selection is done on "total exposure", industry (Agriculture, forestry and fishing plus Financial and insurance activities) and type of firm </t>
+  </si>
+  <si>
+    <t>Goes through how to calibrate a [0, 1] score to probablities of default
+They use scores from  the article 'Approach to the assessment of credit risk for non-financial
+corporations. Evidence from Poland'. This seems to be a logistic regression where the score is the lienar predictor
+It is not clear to me why you take the linear predictor from logistic regression, map it to [0,1] (not using the inverse logit function?) and then use the method they use
+It is not clear to me why you would pull together the industries they do</t>
+  </si>
+  <si>
+    <t>FINANCIAL DISTRESS FORECASTING OF NON-FINANCIAL FIRMS: A CASE OF PAKISTAN</t>
+  </si>
+  <si>
+    <t>Characteristics of firm failure processes in an international context</t>
+  </si>
+  <si>
+    <t>Study 1: 70 firms
+Study 2 and 3: 1216 firms
+Study 4: 1281 firms
+Guess multiple finanical records / period is used in e.g. logistic regression</t>
+  </si>
+  <si>
+    <t>Not stated / I could not find comments about sampling</t>
+  </si>
+  <si>
+    <t>Study 1: Finnish and Estonian 
+Study 2 and 3: European manufacturing firms
+Sutdy 4: Estonia
+See page 46 and 52 for details</t>
+  </si>
+  <si>
+    <t>Applies Zmijewski (1984) logistic model to companies in Pakistian in 2001 to 2010
+The english is bad and the only interest would be that the model is applied to the particular data set. 
+Caveat: I only skimmed the article</t>
+  </si>
+  <si>
+    <t>This is a thesis that summarizes four previous studies. The goal of the studies seems/is descripitve. A large focus is put on the trajectory of failures
+It is interesting with models applied to an international data set
+Use change in accoutning variables. Might be good idea though I figure these should be relative and not abosolute when used in logistic regression 
+Study 2 and 3 may be interesting
+I would argue that 1200-ish firms is not a large sample which the authors claim
+Seems like we have a lot of variables given the figures on page 48 and when you look at the study designs on page 56 plus the sample sizes
+Caveat: I have not read beyond page 57</t>
+  </si>
+  <si>
+    <t>The Research of SME Financial Crisis Warning Model Based on Neural Network</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>Chinece 'SMEs listed in the stock markets in Shanghai and Shenzhen from 2011 to 2015'
+Distress is defined as being marked signed ST which means two consecutive years of loss</t>
+  </si>
+  <si>
+    <t>They 'selected' which may imply some sort of sampling</t>
+  </si>
+  <si>
+    <t>748 firms of which 70% is a traning set, 15% is a testing set and 15% is an examining set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accuracy 83% to 95% presumably on a hold-out set </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fit a neaural network to predict the chinece firms that have two consecutive years of losses
+Details about sampling is not presented
+All observations may be bagged including the hold-out which may imply that the longitudinal aspect is ignored
+</t>
+  </si>
+  <si>
+    <t>Distress Risk: An Accelerated Failure Time Survival Analysis Approach</t>
+  </si>
+  <si>
+    <t>US listed firms between 1980 and 2014 obtained from the Compustat/CRSP
+Excludes financial firms
+Failure is defined as 'delisted firms that underwent bankruptcy or liquidation according to both the Compustat and CRSP classification'</t>
+  </si>
+  <si>
+    <t>'… 546 bankruptcy observations, 8,664 other exit firms and an average of 3,874 active firms for each year over the 1980-2014 period, a total of 544250 quarterly firm observations'</t>
+  </si>
+  <si>
+    <t>Similar results to Shumway (2001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They apply an Accelerated Failure time model (particularly a log-logistic distribution). The starting time is when the firm is listed as is applied to the similar data set as Shumway (2001)
+Find only minor improvments to the models in Shumway (2001) and  Campbell et al. (2008) in terms of in-sample AUC and out-sample decile rankings
+A note here is that in my experience the age of the firms does not matter much. Hence, the previous finding is expected
+Draws conclusions on fits where some coeffecients are large in absolute terms (see table 6). I guess it is a result of multicollinearity </t>
+  </si>
+  <si>
+    <t>My rating (1: best, 5: worst)</t>
+  </si>
+  <si>
+    <t>ACF, LOGI, LDA</t>
   </si>
   <si>
     <t>Failing firms are drawn from 2007–2013
@@ -137,15 +475,7 @@
 Firms do have multiple entries
 Unclear if failing firms also appear with financial statements for the year where they do not default
 Mix years / ignores longitudinal aspect
-Unclear what is meant by the different xthYear data sets</t>
-  </si>
-  <si>
-    <t>Chinece firms from China
-Stock Market and Accounting Research Database
-Default indicator is 'specially treated (ST) by China Securities Supervision and Management Committee'</t>
-  </si>
-  <si>
-    <t>My rating (1 = best, 5 = worst)</t>
+Unclear what is meant by the different 'xthYear' data sets (at least to me)</t>
   </si>
 </sst>
 </file>
@@ -181,9 +511,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -500,10 +833,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,7 +864,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>9</v>
@@ -537,10 +873,10 @@
         <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -554,16 +890,16 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="I2" s="1">
         <v>3</v>
@@ -571,60 +907,421 @@
     </row>
     <row r="3" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="I3" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="I4" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I14" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I18" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with more articles
</commit_message>
<xml_diff>
--- a/data/review_data.xlsx
+++ b/data/review_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="143">
   <si>
     <t>Article name</t>
   </si>
@@ -350,10 +350,6 @@
     <t>See 'Probability-of-default curve calibration and the validation of internal rating systems'</t>
   </si>
   <si>
-    <t>See 'Probability-of-default curve calibration and the validation of internal rating systems'
-I only quickly scanned this but what I saw did not seem resonable / worth reading</t>
-  </si>
-  <si>
     <t>None?</t>
   </si>
   <si>
@@ -403,11 +399,6 @@
 Study 2 and 3: European manufacturing firms
 Sutdy 4: Estonia
 See page 46 and 52 for details</t>
-  </si>
-  <si>
-    <t>Applies Zmijewski (1984) logistic model to companies in Pakistian in 2001 to 2010
-The english is bad and the only interest would be that the model is applied to the particular data set. 
-Caveat: I only skimmed the article</t>
   </si>
   <si>
     <t>This is a thesis that summarizes four previous studies. The goal of the studies seems/is descripitve. A large focus is put on the trajectory of failures
@@ -476,6 +467,135 @@
 Unclear if failing firms also appear with financial statements for the year where they do not default
 Mix years / ignores longitudinal aspect
 Unclear what is meant by the different 'xthYear' data sets (at least to me)</t>
+  </si>
+  <si>
+    <t>Applies Zmijewski (1984) logistic model to companies in Pakistian in 2001 to 2010
+The english is bad and the only interest would be that the model is applied to the particular data set as far as I see
+Caveat: I only skimmed the article</t>
+  </si>
+  <si>
+    <t>See 'Probability-of-default curve calibration and the validation of internal rating systems'
+I only quickly scanned this but what I saw did not seem resonable / worth reading given my review of the above article</t>
+  </si>
+  <si>
+    <t>Medium Risk Companies: The Probability of Notching-Up</t>
+  </si>
+  <si>
+    <t>International Journal of Economics and Finance</t>
+  </si>
+  <si>
+    <t>37,560 firm-year observations that span 9,390 individual' with 504 defaulting firms</t>
+  </si>
+  <si>
+    <t>78% accuracy in-sample between the "worst" rating class and the rest as far as I gather</t>
+  </si>
+  <si>
+    <t>Italian firms from 2007-10
+'The sample excludes firms with significant outlier in some of their explanatory variables so that all the observations in the 1st and the 100th percentile are dropped'
+'Default ... is defined as a payment being ninety days or more past due at least once since origination' with data from the Credit register at Crif Spa
+Includes financial statements with 'not less than 5 million euro of total revenues from sales and not more than 50 million euro' with at least 5 years of operations in Italy
+Excludes '... financial firms, public firms, farms and construction firms.'</t>
+  </si>
+  <si>
+    <t>Performs forward stepwise selection with a logistic model for Italian firms. They then map the predicted default rate into 10 rating classes. Classes are then used to look at transitions between classes from year to year. I found the latter part less interesting from a default prediction perspective
+The handling of outliers seems questionable to me. They must exclude a lot of firms?
+The exclussion of financial statements below 5m. euro means that the method is not applicable for firms whos sales drop below the limit in the financial statement before they default</t>
+  </si>
+  <si>
+    <t>A Global Model for Bankruptcy Prediction</t>
+  </si>
+  <si>
+    <t>PloS one</t>
+  </si>
+  <si>
+    <t>Data from 1990-2013 '440 non-financial, quoted companies belonging to three regions: Asia (Japan, South Korea, Singapore and Taiwan), Europe (Austria, Denmark, France, Germany, Ireland, Italy, Luxembourg, Holland, Norway, Portugal, Spain, Sweden, Switzerland and the United Kingdom) and America (Bermuda, Canada and the United States)' from compustat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50-50 split with match sampling on year, country and industry where the match is selected at random </t>
+  </si>
+  <si>
+    <t>220 / 220 firms</t>
+  </si>
+  <si>
+    <t>AUC on hold-out sample of 80% to 93%</t>
+  </si>
+  <si>
+    <t>Fits regional and a global logitistic model with financial data from 1, 2 and 3 years prior to the default
+I find some flaws:
+The study is nice in that it test for regional differences. Though, I see no reason for the sampling when they use logistic regression
+Small samples with with 10 variables
+Infers that there is regional differences based on different selected variables in the regional model where the model is selected that minimize an information criteria (Hannan-Quinn criteria) which I guess is seleted with stepwise selection or similar
+Matched sampling
+Bag all observations across years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firms from Belgium, France, Greece, Italy, the Netherlands, Portugal, or Spain in the ORBIS, a database of Bureau van Dijk
+Data is from 2004-13 excluding 2010
+From one of these industry: ‘Construction’, ‘Machinery, equipment, furniture, recycling’, ‘Metals &amp; metal products’, ‘Other services’, or ‘Wholesale &amp; retail trade’
+See page 34 for further criterias
+</t>
+  </si>
+  <si>
+    <t>AUC ranging from 34% to 92% on hold-out samples</t>
+  </si>
+  <si>
+    <t>1991 firms in their 2004-06 sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compares linear discrimation analysis, logistic regression and probit models for European firms
+Compares inter and intra industry models
+Estimates the model over three periods
+Scale ratio by inverse of industry ratios
+Includes macro economic variables
+I am not convinced that their yearly strafied sampling of a 10:1 ratio is a good way to do it
+The absolotue value of the estimated coeffecients seems quite large. I guess it is a cause of multicollinearity
+The authors lost me with their 31 tables and 4 page conclussion </t>
+  </si>
+  <si>
+    <t>Forecasting European Corporate Bankruptcy</t>
+  </si>
+  <si>
+    <t>A 10-1 ratio which I guess is random. Though ' A minimum of 200 healthy firms' in each year. See page 34 for further details</t>
+  </si>
+  <si>
+    <t>Bankruptcy Prediction Using Memetic Algorithm</t>
+  </si>
+  <si>
+    <t>Use a 'new memetic algorithm using Cuckoo search algorithm and Particle Swarm optimization algorithm' to train classifiers of sets of data of banks
+It is not clear what data they are using and how it is sample
+They do not get a consistent better result with accurarcy relative to a decision tree</t>
+  </si>
+  <si>
+    <t>International Workshop on Multi-disciplinary Trends</t>
+  </si>
+  <si>
+    <t>AUCs of 73% (in sample?)</t>
+  </si>
+  <si>
+    <t>532 / 90729 financial statements with 23326 unique firms</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Why Do Companies Fail</t>
+  </si>
+  <si>
+    <t>Estimates a discrete cox regression (that is use the cloglog function in binary regression). The underlying time variable is set to the log of age of the firm times a constant from what I gather. Age is 'measured as the natural log of the number of years since the company registered with Default indicator is from Australian Securities and Investments Commission'
+Notice that adding a year dummy to a discrete Cox regression is essentially semi parametric cox regression where the underlying time process is the calender time 
+Compares estimates from listed and non-listed firms that are modeled seperatly 
+Has a large sample of both firms
+Has some nice Kaplan-Meier Failure Curves for age strafied by private, public listed or public not listed</t>
+  </si>
+  <si>
+    <t>Australian firm both private, public listed and public non-listed
+Data for listed firms is for firms on the Australian Stock Exchange from Morningstar
+Data for unlisted firms is from Dun &amp; Bradstreet
+Default indicator is from Australian Securities and Investments Commission
+Some removal of imposible values is performed - see page 13</t>
+  </si>
+  <si>
+    <t>LOGI, LDA</t>
   </si>
 </sst>
 </file>
@@ -511,12 +631,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -833,13 +956,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,7 +996,7 @@
         <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="144" x14ac:dyDescent="0.3">
@@ -948,7 +1071,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>22</v>
@@ -1171,19 +1294,19 @@
         <v>77</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="I12" s="1">
         <v>5</v>
@@ -1197,7 +1320,7 @@
         <v>77</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>51</v>
@@ -1206,7 +1329,7 @@
         <v>81</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I13" s="1">
         <v>5</v>
@@ -1229,7 +1352,7 @@
         <v>83</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="I14" s="1">
         <v>5</v>
@@ -1237,13 +1360,13 @@
     </row>
     <row r="15" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="I15" s="1">
         <v>5</v>
@@ -1251,22 +1374,22 @@
     </row>
     <row r="16" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="I16" s="1">
         <v>5</v>
@@ -1274,25 +1397,25 @@
     </row>
     <row r="17" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="I17" s="1">
         <v>3</v>
@@ -1300,28 +1423,155 @@
     </row>
     <row r="18" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="I18" s="1">
         <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I19" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I20" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I22" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I23" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update of reviews + added abstract to html page
</commit_message>
<xml_diff>
--- a/data/review_data.xlsx
+++ b/data/review_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15192" windowHeight="5688"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7656" windowHeight="5688"/>
   </bookViews>
   <sheets>
     <sheet name="review_data" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="192">
   <si>
     <t>Article name</t>
   </si>
@@ -195,12 +195,6 @@
   </si>
   <si>
     <t>At best 80% accuracy (in-sample?)</t>
-  </si>
-  <si>
-    <t>They compare different ways of accountning for time-varying effects with neural networks. In essence, they use data in slidding window for their best model. Further, they apply an ensamble method where variables in each fit is random 
-It is nice that they account for the longitudinal aspect of data 
-Getting at best 80% accuracy (in-sample?) with a small data set with neural networks and 36 variables seems too low when further considering that we are looking at listed firms. Hence, data should be rather "clean"/homogeneous
-Paired sample</t>
   </si>
   <si>
     <t>Additive Intensity Regression Models in Corporate Default Analysis</t>
@@ -367,12 +361,6 @@
     <t>20 / 44 where there is a 50%-50% split to in training</t>
   </si>
   <si>
-    <t xml:space="preserve">Polish firms from 2007 to 2012
-Defaults from Narodowy Bank Polski and National Court Register (KRS)
-Financial data from AMADEUS (Bureau van Dijk); Notoria OnLine
-Some selection is done on "total exposure", industry (Agriculture, forestry and fishing plus Financial and insurance activities) and type of firm </t>
-  </si>
-  <si>
     <t>Goes through how to calibrate a [0, 1] score to probablities of default
 They use scores from  the article 'Approach to the assessment of credit risk for non-financial
 corporations. Evidence from Poland'. This seems to be a logistic regression where the score is the lienar predictor
@@ -487,19 +475,11 @@
     <t>37,560 firm-year observations that span 9,390 individual' with 504 defaulting firms</t>
   </si>
   <si>
-    <t>78% accuracy in-sample between the "worst" rating class and the rest as far as I gather</t>
-  </si>
-  <si>
     <t>Italian firms from 2007-10
 'The sample excludes firms with significant outlier in some of their explanatory variables so that all the observations in the 1st and the 100th percentile are dropped'
 'Default ... is defined as a payment being ninety days or more past due at least once since origination' with data from the Credit register at Crif Spa
 Includes financial statements with 'not less than 5 million euro of total revenues from sales and not more than 50 million euro' with at least 5 years of operations in Italy
 Excludes '... financial firms, public firms, farms and construction firms.'</t>
-  </si>
-  <si>
-    <t>Performs forward stepwise selection with a logistic model for Italian firms. They then map the predicted default rate into 10 rating classes. Classes are then used to look at transitions between classes from year to year. I found the latter part less interesting from a default prediction perspective
-The handling of outliers seems questionable to me. They must exclude a lot of firms?
-The exclussion of financial statements below 5m. euro means that the method is not applicable for firms whos sales drop below the limit in the financial statement before they default</t>
   </si>
   <si>
     <t>A Global Model for Bankruptcy Prediction</t>
@@ -596,6 +576,209 @@
   </si>
   <si>
     <t>LOGI, LDA</t>
+  </si>
+  <si>
+    <t>Predicting corporate failure in Zambia: A case of manufacturing firms</t>
+  </si>
+  <si>
+    <t>IJAR</t>
+  </si>
+  <si>
+    <t>Logistic regression with firms from Zambia
+A very small sample
+Caveat: I only skimmed the article</t>
+  </si>
+  <si>
+    <t>'Norwegian limited liability firms in the period 1996–2001'</t>
+  </si>
+  <si>
+    <t>GAM, NN, LOGI, LDA</t>
+  </si>
+  <si>
+    <t>'… approximately 100 000 firms each year only about 1% defaulted the next year'</t>
+  </si>
+  <si>
+    <t>Models defaults using generalized aditive models in Norway with a large set of firms
+Models different default horizonts
+Finds imporvments of using generalized additve models over linear discrimination, logistic regression and neural networks 
+A large sample is used
+Use change variables from previous year which may be a good idea. I am not sure whether it is a good idea to use the industry means for the first year of data
+Details about this comment would be useful:' In a preliminary analysis we removed variables that were not significant in any model'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Up to 78% AUC on out-sample in time </t>
+  </si>
+  <si>
+    <t>Performs forward stepwise selection with a logistic model for Italian firms. They then map the predicted default rate into 10 rating classes. Classes are then used to look at transitions between classes from year to year. I found the latter part less interesting from a default prediction perspective
+The handling of outliers seems questionable to me. They must exclude a lot of firms?</t>
+  </si>
+  <si>
+    <t>Applied Stochastic Models in Business and Industr</t>
+  </si>
+  <si>
+    <t>Bankruptcy prediction by generalized additive models</t>
+  </si>
+  <si>
+    <t>17,570 firms and 1,571,115 firm-months with 1383 bankruptcy filings</t>
+  </si>
+  <si>
+    <t>US (listed?) firms in the the year 1980-2009
+Data from Center for Research in Security Prices (CRSP) with annual financial information from COMPUSTAT.
+Use chapter 7 or chapter 11 as a default indicator</t>
+  </si>
+  <si>
+    <t>1 year a-head out-sample forecast AUC of 84%</t>
+  </si>
+  <si>
+    <t>Performs an logistic regression with Lasso (L1) penalty with data from the US. Find improvements in relative to the model in Campbell et al (2008)
+I do not think to conclusions should be drawn on which covariate are selected when multicollinearity is present. As far as I re-call, the selection properties of Lasso regression is ussually driven under the assumption of orthogonal design matricies for good reasons</t>
+  </si>
+  <si>
+    <t>Variable selection and corporate bankruptcy forecasts</t>
+  </si>
+  <si>
+    <t>Journal of Banking &amp; Finance</t>
+  </si>
+  <si>
+    <t>Random sampling is performed with equal split between benkerupt and non-bankerupt firms</t>
+  </si>
+  <si>
+    <t>Up to 1100 / 1100</t>
+  </si>
+  <si>
+    <t>One year a-head out-sample in time accurarcy of 80%-81%</t>
+  </si>
+  <si>
+    <t>Forecasting financial failure using a Kohonen map: A comparative study to improve model stability over time</t>
+  </si>
+  <si>
+    <t>European Journal of Operational Research</t>
+  </si>
+  <si>
+    <t>French firms between 1991-2009 from the database Diane
+Only firms required to '… file their annual reports with the French commercial courts' are included
+Firms are selected from the retail industry 
+With total assets less than €750000 (in all periods?)
+Companies that are operating for at least 6 years</t>
+  </si>
+  <si>
+    <t>I assume that the failed firms must be sampled or selected from the entire population
+Paired sample based oon indstry and asset size</t>
+  </si>
+  <si>
+    <t>78 / 78 firms with one financial statement from each firm</t>
+  </si>
+  <si>
+    <t>US firms in the perio 1954-64
+Excludes firm of noncorporate form, privately held corporations, and nonindustrial firms
+'… bankrupt firms provided by Dun and Bradstre' or Moody's
+'the financial statements could not be more than six months old at the date of failure'</t>
+  </si>
+  <si>
+    <t>Performs univariate analysis of US firms
+While the paper is highly cited the paper is also dated. I say there is little compared to other papers</t>
+  </si>
+  <si>
+    <t>Financial ratios as predictors of failure</t>
+  </si>
+  <si>
+    <t>Journal of accounting research</t>
+  </si>
+  <si>
+    <t>50-50 split where the sampling is not clear to me. I guess it is random given the comment on page 100</t>
+  </si>
+  <si>
+    <t>Manualy gathered of Hungarian firms with data available over the 2001-2012
+Benkerupt firms are taken as those under liquidation or bankruptcy proceeding. The source is Hungarian Trade Register 
+'Companies which hadn’t been realizing sales for at least two consecutive years were also excluded from the experiment'
+See page 100 for further criteria</t>
+  </si>
+  <si>
+    <t>At most 1000 firms with 7592 financial statements</t>
+  </si>
+  <si>
+    <t>75%-80% accuracy with 10 fold cross validation</t>
+  </si>
+  <si>
+    <t>This is a Ph.D. thesis for a study of  bankruptcy prediction
+It provides are good framework for formalizing the model building (see page 26) with a comprehensive literature review of each step. There is 20 pages of references which stress the latter point 
+Quite readable 
+One can skip the study though as:
+I find that this is one of the best introduction into bankeruptcy prediction although it is long
+I am not convinced that the dynamic variables introduced on page 92 is good idea. I assume they will be quite unstable for firms with little prior data (which motivaties the treatment of outliers later). They do not seem useful to when you look at the results at table 113
+Excluding 'Companies which hadn’t been realizing sales for at least two consecutive' may not a be a good idea
+The treatment of outliers seems questionable to me. Any covariate outsite +/- 2 standard deviations seems like an bad definition</t>
+  </si>
+  <si>
+    <t>APPLICATION OF DYNAMIC FINANCIAL VARIABLES IN BANKRUPTCY PREDICTION</t>
+  </si>
+  <si>
+    <t>Aggregating multiple classification results using Choquet integral for financial distress early warning</t>
+  </si>
+  <si>
+    <t>Classifiers selection in ensembles using genetic algorithms for bankruptcy prediction</t>
+  </si>
+  <si>
+    <t>Two-level classifier ensembles for credit risk assessment</t>
+  </si>
+  <si>
+    <t>Development of a class of stable predictive variables: The case of bankruptcy prediction</t>
+  </si>
+  <si>
+    <t>Journal of Business Finance &amp; Accounting</t>
+  </si>
+  <si>
+    <t>SMR, LOGI, LDA, CM, NN</t>
+  </si>
+  <si>
+    <t>Financial distress prediction with classifier ensembles based on firm life cycle and Choquet integral</t>
+  </si>
+  <si>
+    <t>Clustering and visualization of bankruptcy trajectory using self-organizing map</t>
+  </si>
+  <si>
+    <t>They compare different ways of accountning for time-varying effects with neural networks. In essence, they use data in slidding window for their best model. Further, they apply an ensamble method where variables in each fit is random 
+It is nice that they account for the longitudinal aspect of data 
+Getting at best 80% accuracy (in-sample?) with a small data set with neural networks and 36 variables seems too low when further considering that we are looking at listed firms. Hence, data should be rather 'clean'/homogeneous
+Paired sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polish firms from 2007 to 2012
+Defaults from Narodowy Bank Polski and National Court Register (KRS)
+Financial data from AMADEUS (Bureau van Dijk); Notoria OnLine
+Some selection is done on 'total exposure' industry (Agriculture, forestry and fishing plus Financial and insurance activities) and type of firm </t>
+  </si>
+  <si>
+    <t>78% accuracy in-sample between the 'worst' rating class and the rest as far as I gather</t>
+  </si>
+  <si>
+    <t>Try Kohonen maps in forecasting of bankeruptcy. As I gather, this implies a mapping into a 2D grid followed by an anlysis of firm trajectories on the map
+The idea seems to be a good visual tool although I am not convinced that the method is superior to other methods
+Selection of variables is done with some of the comparisson models with backward search 
+I don’t think the comparisson between the other models and the Koherent map is fair. There is 'way' more data avialable for the 1 year for these methods which seems not to be used (see section 3.5). This may explain why the cox model gets better result than the logistic regression
+It is not clear to me how firms that default in intermediate years of the estimations period is used
+The requirement of 6 consequetive years of data may be an issue</t>
+  </si>
+  <si>
+    <t>Predicting Financial Distress: Multi Scenarios Modeling Using Neural Network</t>
+  </si>
+  <si>
+    <t>Fits a neural network with only 37 firms from the Egyptian stock exchange. 82 financial statements are excluded due to missing variables
+Firms a sampled though I could not figure out the details
+Caveat: I only skimmed the article</t>
+  </si>
+  <si>
+    <t>(In sample?) AUC between 83%-91%</t>
+  </si>
+  <si>
+    <t>LOGI, CM</t>
+  </si>
+  <si>
+    <t>Master thesis studying 627 high-yield bonds in the period of 2006-14. 126 of these default. Uses logistic regression and Cox regression with stepwise model selection
+Small sample</t>
+  </si>
+  <si>
+    <t>Default in the Nordic High-Yield Bond Market</t>
   </si>
 </sst>
 </file>
@@ -631,7 +814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -640,6 +823,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -956,13 +1142,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,7 +1182,7 @@
         <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="144" x14ac:dyDescent="0.3">
@@ -1071,7 +1257,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>22</v>
@@ -1138,7 +1324,7 @@
         <v>45</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>46</v>
+        <v>182</v>
       </c>
       <c r="I6" s="1">
         <v>5</v>
@@ -1146,28 +1332,28 @@
     </row>
     <row r="7" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="I7" s="1">
         <v>2</v>
@@ -1175,28 +1361,28 @@
     </row>
     <row r="8" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I8" s="1">
         <v>1</v>
@@ -1204,28 +1390,28 @@
     </row>
     <row r="9" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="I9" s="1">
         <v>3</v>
@@ -1233,25 +1419,25 @@
     </row>
     <row r="10" spans="1:9" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="I10" s="1">
         <v>2</v>
@@ -1259,28 +1445,28 @@
     </row>
     <row r="11" spans="1:9" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="I11" s="1">
         <v>3</v>
@@ -1288,25 +1474,25 @@
     </row>
     <row r="12" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="D12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="I12" s="1">
         <v>5</v>
@@ -1314,22 +1500,22 @@
     </row>
     <row r="13" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="H13" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I13" s="1">
         <v>5</v>
@@ -1337,22 +1523,22 @@
     </row>
     <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I14" s="1">
         <v>5</v>
@@ -1360,13 +1546,13 @@
     </row>
     <row r="15" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I15" s="1">
         <v>5</v>
@@ -1374,22 +1560,22 @@
     </row>
     <row r="16" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="I16" s="1">
         <v>5</v>
@@ -1397,25 +1583,25 @@
     </row>
     <row r="17" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="I17" s="1">
         <v>3</v>
@@ -1423,25 +1609,25 @@
     </row>
     <row r="18" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="H18" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="I18" s="1">
         <v>4</v>
@@ -1449,28 +1635,28 @@
     </row>
     <row r="19" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>117</v>
+        <v>184</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
       <c r="I19" s="1">
         <v>4</v>
@@ -1478,28 +1664,28 @@
     </row>
     <row r="20" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="I20" s="1">
         <v>4</v>
@@ -1507,25 +1693,25 @@
     </row>
     <row r="21" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I21" s="1">
         <v>5</v>
@@ -1533,16 +1719,16 @@
     </row>
     <row r="22" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I22" s="1">
         <v>5</v>
@@ -1550,28 +1736,266 @@
     </row>
     <row r="23" spans="1:9" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="I23" s="1">
         <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I24" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I25" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I26" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I27" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I28" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I36" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I37" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit before I start to play around with table sorter
</commit_message>
<xml_diff>
--- a/data/review_data.xlsx
+++ b/data/review_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="226">
   <si>
     <t>Article name</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>LDA, NN, AdaBoost</t>
-  </si>
-  <si>
-    <t>Data source</t>
   </si>
   <si>
     <t>Spanish firms from the SABI database of Bureau Van Dijk</t>
@@ -613,9 +610,6 @@
 The handling of outliers seems questionable to me. They must exclude a lot of firms?</t>
   </si>
   <si>
-    <t>Applied Stochastic Models in Business and Industr</t>
-  </si>
-  <si>
     <t>Bankruptcy prediction by generalized additive models</t>
   </si>
   <si>
@@ -779,6 +773,152 @@
   </si>
   <si>
     <t>Default in the Nordic High-Yield Bond Market</t>
+  </si>
+  <si>
+    <t>Predicting bankruptcy in European e-commerce sector</t>
+  </si>
+  <si>
+    <t>LOGI, DT, CL</t>
+  </si>
+  <si>
+    <t>Small sample of 124 companies of European E commerce retailers. Data spans up to 2014. Applies different method to predict the outcome
+An almost 48%-52% sample is made. I cannot find details about the sampling
+I see no reason to sample with the methods they use</t>
+  </si>
+  <si>
+    <t>16929 observations which I guess is financial statements</t>
+  </si>
+  <si>
+    <t>None as far as I gather</t>
+  </si>
+  <si>
+    <t>Compares logistic models on US data where one include a binary variable from the Credit Initiative predicted probability of default (see page 34) and the other includes a indicator for going concern opinions (GCOs)
+It is not clear to me why you make this comparisson and include the binary variable they do. Why not test the Credit Initiative model directly?
+It may be that they only use firms who do eventually default? I guess so from page 17 with the notion of distressed firm-years and the section on page 26</t>
+  </si>
+  <si>
+    <t>AUC of 87%-89% using cross validation</t>
+  </si>
+  <si>
+    <t>How useful are auditors’ going concern opinions as predictors of default?</t>
+  </si>
+  <si>
+    <t>US companies in 2000-12
+Default data is from 'the database of the Credit Research Initiative (CRI)'
+Accounting data is from  Compustat North America with audit data from  Audit Analytics
+Excludes financial firms
+Use a hard and soft defintion of failure (see page 15)</t>
+  </si>
+  <si>
+    <t>'3,960 firm year observations for the bankrupt sample; and 26,169 firm year observations for the ... non-failed group'</t>
+  </si>
+  <si>
+    <t>AUC from 74%-93% computed with cross validation</t>
+  </si>
+  <si>
+    <t>It is unclear to me if the controls are sampled. See page 11</t>
+  </si>
+  <si>
+    <t>US public company
+Default data is from 'Standard’s and Poor Capital IQ service.'
+'collected up to three years of financial variables on all bankrupt firms prior to the year of bankruptcy'
+They 'code previous years [in plural] of a bankrupt firm as bankrupt. For instance, if a company failed in 2013, and three preceding years of financial data exists on that firm, all years are coded as ‘0’ or bankrupt.'
+Chapter 11 filling is used as the definition of failure
+It is not clear to me how the accounting data is selected for the non-failing firms. See page 11 ('We extracted the same data for the non-failed control sample')</t>
+  </si>
+  <si>
+    <t>PREDICTING CORPORATE BANKRUPTCY: AN EVALUATION OF ALTERNATIVE STATISTICAL FRAMEWORKS</t>
+  </si>
+  <si>
+    <t>Journal of Business Finance</t>
+  </si>
+  <si>
+    <t>B, LOGI, SVM, RF, SVM, AdaBoost, NN</t>
+  </si>
+  <si>
+    <t>A study that compares a varity of methods on US pulically listed firms
+Seems to suggest that the ensamble methods are preferable
+Box cox transform variables. Seems only to matter for the models that do depend on monotonic transformation as expected
+Tries with missing value imputation using an SVM method. The performance does not change 
+Lags details of sampling of non-failing firms and the
+I am not convienced that the marking all three prior years as failure is a good idea - especially if they do let the defaulting firms be control in any other periods
+Note that they addresss the prevoius point on page 28 under the header 'Look-ahead bias. ' Further, you loose a lot of data this way. The failing firms would have been active healthy firms for while before defaulting</t>
+  </si>
+  <si>
+    <t>Data source/set</t>
+  </si>
+  <si>
+    <t>US firms listed on NYSE,AMEX, and NASDAQ exchanges in the period 1980-93
+Compustat is used for financial statements
+LEXIS/NEXIS database is used for exit type
+Randomly selected sixteen three-digit SIC code industries 
+'an early warning signal' was present in the period 1980 to 1988. They used the Alman Z-score for this purpose
+Imputes industry median or zeros for missing values. See page 5</t>
+  </si>
+  <si>
+    <t>European Management Review</t>
+  </si>
+  <si>
+    <t>More than a Dummy: The Probability of Failure, Survival and Acquisition of Firms in Financial Distress</t>
+  </si>
+  <si>
+    <t>US firms listed on NYSE and AMEX between 1980-2006
+Data is from New Generation Research (www.bankruptcydata.com), Compustat and CRSP
+Use chapter 11 as the default outcome
+Excludes firms with missing values and financial firms and those with SIC greater than 5999</t>
+  </si>
+  <si>
+    <t>Test previous model specification for logit models on similar data sets in the US
+Adds a variable for the 'number of separate business segments in each of our sample firms'
+Adds a lagged version of some of the variables
+I would assumet that this action would make their result artifically high. Firms that exit for other reason could likely be similar to firms that default:' We exclude firms that are delisted from CRSP or deleted from Compustat for reasons other than bankruptcy or liquidation'
+This is just stupid. Of course the test gets better in sample as the firms that fail are likely similar a few years prior. Though, you would not know this berfore hand. This comment is for '[our is model] equivalent ... Shumway[s] (2001) [model], except that we only include one firm-year observation for each bankrupt firm but all firm-year observations for the surviving firm. This refinement significantly improves model performance.'</t>
+  </si>
+  <si>
+    <t>887 bankruptcies and 49,724 non-bankrupt firm-years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUC of 93% though see the my review </t>
+  </si>
+  <si>
+    <t>Journal of Contemporary Accounting &amp; Economics</t>
+  </si>
+  <si>
+    <t>A comparison of alternative bankruptcy prediction models</t>
+  </si>
+  <si>
+    <t>'... we randomly select 500 firms from the identified active-firm-pool for each sample year. Once a non-bankrupt firm is selected for a year, it is excluded from selection in later years'</t>
+  </si>
+  <si>
+    <t>890 / 6932 financial statements</t>
+  </si>
+  <si>
+    <t>Around 81% accurarcy using cross validation</t>
+  </si>
+  <si>
+    <t>SVM, LOGI</t>
+  </si>
+  <si>
+    <t>Firms traded on publicly NASDAQ
+'bankrupt firms are identified through Compustat and Lexis–Nexis Bankruptcy Report'
+It seems that bankerupt firms are only included as with their latest financial statement (see page 742)
+A few firms with missing values are deleted with all missing variables</t>
+  </si>
+  <si>
+    <t>Use Bayes Bayesian network for US listed firms
+An advantage of these methods is that the methods can deal with missing values as they show
+Show improvements relative to a logistic regression. I speculate that the improvements would not be present if they dealt with extremes values (see the descriptive statistics in table 2)
+It is problematic if firms that do fail are not included in the years where they do not fail as controls</t>
+  </si>
+  <si>
+    <t>Using Bayesian networks for bankruptcy prediction: Some methodological issues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While I do find multi exit models interesting (which they model) I have no idea why they only define 'survivers' as those who goes below a certain Altman Z-score. Why not extend the idea Shumway (2001) into a multinomial model?
+Either their ROC curves turns mirrored or their performance is horriable (see page 14)... </t>
+  </si>
+  <si>
+    <t>Applied Stochastic Models in Business and Industry</t>
   </si>
 </sst>
 </file>
@@ -1142,13 +1282,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A38" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1167,22 +1307,22 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>207</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="144" x14ac:dyDescent="0.3">
@@ -1196,19 +1336,19 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="1">
         <v>3</v>
@@ -1216,28 +1356,28 @@
     </row>
     <row r="3" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I3" s="1">
         <v>5</v>
@@ -1245,28 +1385,28 @@
     </row>
     <row r="4" spans="1:9" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I4" s="1">
         <v>2</v>
@@ -1274,28 +1414,28 @@
     </row>
     <row r="5" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I5" s="1">
         <v>3</v>
@@ -1303,28 +1443,28 @@
     </row>
     <row r="6" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I6" s="1">
         <v>5</v>
@@ -1332,28 +1472,28 @@
     </row>
     <row r="7" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="I7" s="1">
         <v>2</v>
@@ -1361,28 +1501,28 @@
     </row>
     <row r="8" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="D8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I8" s="1">
         <v>1</v>
@@ -1390,28 +1530,28 @@
     </row>
     <row r="9" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="I9" s="1">
         <v>3</v>
@@ -1419,25 +1559,25 @@
     </row>
     <row r="10" spans="1:9" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="I10" s="1">
         <v>2</v>
@@ -1445,28 +1585,28 @@
     </row>
     <row r="11" spans="1:9" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="I11" s="1">
         <v>3</v>
@@ -1474,25 +1614,25 @@
     </row>
     <row r="12" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="D12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="I12" s="1">
         <v>5</v>
@@ -1500,22 +1640,22 @@
     </row>
     <row r="13" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="H13" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I13" s="1">
         <v>5</v>
@@ -1523,22 +1663,22 @@
     </row>
     <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I14" s="1">
         <v>5</v>
@@ -1546,13 +1686,13 @@
     </row>
     <row r="15" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I15" s="1">
         <v>5</v>
@@ -1560,22 +1700,22 @@
     </row>
     <row r="16" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="I16" s="1">
         <v>5</v>
@@ -1583,25 +1723,25 @@
     </row>
     <row r="17" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="I17" s="1">
         <v>3</v>
@@ -1609,25 +1749,25 @@
     </row>
     <row r="18" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="I18" s="1">
         <v>4</v>
@@ -1635,28 +1775,28 @@
     </row>
     <row r="19" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I19" s="1">
         <v>4</v>
@@ -1664,28 +1804,28 @@
     </row>
     <row r="20" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="I20" s="1">
         <v>4</v>
@@ -1693,25 +1833,25 @@
     </row>
     <row r="21" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="F21" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F21" s="3" t="s">
+      <c r="H21" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="I21" s="1">
         <v>5</v>
@@ -1719,16 +1859,16 @@
     </row>
     <row r="22" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="I22" s="1">
         <v>5</v>
@@ -1736,25 +1876,25 @@
     </row>
     <row r="23" spans="1:9" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="I23" s="1">
         <v>3</v>
@@ -1762,16 +1902,16 @@
     </row>
     <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="I24" s="1">
         <v>5</v>
@@ -1779,28 +1919,28 @@
     </row>
     <row r="25" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="I25" s="1">
         <v>3</v>
@@ -1808,28 +1948,28 @@
     </row>
     <row r="26" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="I26" s="1">
         <v>3</v>
@@ -1837,28 +1977,28 @@
     </row>
     <row r="27" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="E27" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="H27" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I27" s="1">
         <v>4</v>
@@ -1866,25 +2006,25 @@
     </row>
     <row r="28" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="I28" s="1">
         <v>4</v>
@@ -1892,25 +2032,25 @@
     </row>
     <row r="29" spans="1:9" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="I29" s="1">
         <v>1</v>
@@ -1918,64 +2058,64 @@
     </row>
     <row r="30" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I36" s="1">
         <v>5</v>
@@ -1983,19 +2123,166 @@
     </row>
     <row r="37" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="I37" s="1">
         <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I38" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I39" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I40" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I41" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I42" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I43" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated review data and made fixed error when the journal url is empty
</commit_message>
<xml_diff>
--- a/data/review_data.xlsx
+++ b/data/review_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="349">
   <si>
     <t>Article name</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t>A Combination Use of Bagging and Random Subspace with Memory Mechanism for Dynamic Financial Distress Prediction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Industrial Engineering and Engineering Management </t>
   </si>
   <si>
     <t>NN, B</t>
@@ -278,9 +275,6 @@
     <t>Modelling The Credit Risk Of The Hungarian Sme Sector</t>
   </si>
   <si>
-    <t>mnb</t>
-  </si>
-  <si>
     <t>Up to 2629468 financial statements and 173664 firms</t>
   </si>
   <si>
@@ -301,9 +295,6 @@
   </si>
   <si>
     <t>A Failure-Rate Model for the Danish Corporate Sector</t>
-  </si>
-  <si>
-    <t>Asia-Pacific Journal of Risk and Insurance</t>
   </si>
   <si>
     <t>Probability-of-default curve calibration and the validation of internal rating systems</t>
@@ -769,9 +760,6 @@
     <t>AUC of 87%-89% using cross validation</t>
   </si>
   <si>
-    <t>How useful are auditors’ going concern opinions as predictors of default?</t>
-  </si>
-  <si>
     <t>US companies in 2000-12
 Default data is from 'the database of the Credit Research Initiative (CRI)'
 Accounting data is from  Compustat North America with audit data from  Audit Analytics
@@ -1100,9 +1088,6 @@
   </si>
   <si>
     <t>Some new models for financial distress prediction in the UK</t>
-  </si>
-  <si>
-    <t>Xfi-Centre for Finance and Investment</t>
   </si>
   <si>
     <t>Default prediction with dynamic sectoral and macroeconomic frailties</t>
@@ -1271,6 +1256,161 @@
   </si>
   <si>
     <t>Computers &amp; Operations Research</t>
+  </si>
+  <si>
+    <t>Dynamics of firm financial evolution and bankruptcy prediction</t>
+  </si>
+  <si>
+    <t>Ensemble with neural networks for bankruptcy prediction</t>
+  </si>
+  <si>
+    <t>AUCs up to 76% using 10 fold cross validation</t>
+  </si>
+  <si>
+    <t>Not clear. There is a total of 1458 firms</t>
+  </si>
+  <si>
+    <t>NN, AdaBoost, BA</t>
+  </si>
+  <si>
+    <t>'The data set contains 1458 externally audited manufacturing firms, half of which went bankrupt during 2002–2005 while healthy firms were selected from active companies at the end of 2005'</t>
+  </si>
+  <si>
+    <t>It is not clear. I figure they must have used a skewed sample since they use binary results and given their Type I and II errors in table 6</t>
+  </si>
+  <si>
+    <t>A note on the use of industry-relative ratios in bankruptcy prediction</t>
+  </si>
+  <si>
+    <t>Paired sampling where '… each bankrupt firm was paired with a nonfailed company having the same four digit SIC code, nearly equal asset size, and data for the same year.'</t>
+  </si>
+  <si>
+    <t>67 / 67 for estimation and 34 / 34 for testing</t>
+  </si>
+  <si>
+    <t>Out-sample (in time) accuracies of 86%</t>
+  </si>
+  <si>
+    <t>Compares financial ratios with financial ratios relative to the industry average of the ratio. Industries are defined as 4 digit SIC
+Find that coeffecients are more stable with the industry relative ratios
+Gets better out-sample results with industry relative ratios
+Industry relative ratios may be a good idea. However, this is a small sample with paired sampling so I am reluctant to draw conclusions based on this paper</t>
+  </si>
+  <si>
+    <t>US traded firms
+Traning data consist of '114 equally matched bankrupt and nonfailed' in the period 1972 to 3. quater of 1986
+Default events is taken from Compustat and SEC from frims that 'filed bankruptcy petitions (but did not liquidate)' 
+Out sample data is taken in a similar manner with data from 4. quater of 1986 to 1987
+Industry averages are computed with data from Compustat</t>
+  </si>
+  <si>
+    <t>Multivariate Ordinal Regression Models: An Analysis of Corporate Credit Ratings</t>
+  </si>
+  <si>
+    <t>Dynamic forecasting of financial distress: the hybrid use of incremental bagging and genetic algorithm—empirical study of Chinese listed corporations</t>
+  </si>
+  <si>
+    <t>'NYSE and AMEX-listed Compustat firms. Bankrupt firms were identified through a variety of sources including the 2003 Compustat Annual Industrials file, the 2003 CRSP Monthly Stock file, the website Bankruptcy.com, the Capital Changes Reporter, and a list of firms generously supplied by Shumway'
+Excludes financial or utility industries</t>
+  </si>
+  <si>
+    <t>544 / 4,237 firms with 74,823 firm years</t>
+  </si>
+  <si>
+    <t>Only reports in-sample and out-sample deciles ranking. Results are comparable to Shumway (2001)</t>
+  </si>
+  <si>
+    <t>AdaBoost, SMR, SVM, DT</t>
+  </si>
+  <si>
+    <t>AdaBoost ensemble for financial distress prediction: An empirical comparison with data from Chinese listed companies</t>
+  </si>
+  <si>
+    <t>'Healthy companies are chosen from those that have never been specially treated by the matching method considering both industry and asset size'</t>
+  </si>
+  <si>
+    <t>30 times holdout with 2/3 used in estimation and 1/3 used for testing. The mean hold out testing error for one year is 2.78%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uses Adaboost with decision trees and single attribute test (kind of like univariate discriminant in Beaver (1966)) for predicting distress for Chinese listed firm. Compare the results with SVM and a single decision tree
+Ignores the longitudinal aspect of data by bagging all observations and (potentially) only using one observation from each firm (it is not clear to me if the latter is true or not)
+I figure that 41 variables in SVM with potentially redundant ones could affact the SVM performs a lot - especially in small sample
+Finds that Adaboost performs best and particularly with single attribute test. While this is interesting I, it is hard to draw definitive conclusion due to some of the remarks above and the fact that paired sampling is used </t>
+  </si>
+  <si>
+    <t>692 companies in what I gather is a 50-50 split</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chinese listed firms from 2000 to 2008
+'Financially distressed company is defined as the one who has had negative net profit in consecutive two years'. These firms are referred to as specially treated </t>
+  </si>
+  <si>
+    <t>Does Corporate Governance Affect the Financial Distress of Indonesian Company? A Survival Analysis Using Cox Hazard Model with Time-Dependent Covariates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">600 / 600 firms where I figure only one set of accountning data is selected from each firm </t>
+  </si>
+  <si>
+    <t>AdaBoost, BA, DT, SMR, SVM, NN</t>
+  </si>
+  <si>
+    <t>Uses ensamble learning with descision tress to predict failure for Korean firms. Propose and use a genetic algorithm to reduce the ensamble which uses the variance inflation factor in the fitness function
+The genetic algorithm may or may not be a good idea. I am not sure why they use the variance inflation factor. There are other meassures of diversity which I have seen is more commonly used in ensamble learning. Moreover, I am not sure that optimizing diversity rather than performance is a good idea
+A 75% AUC simply by sorting by total assets seems to me like there is a selecting effect in the data (see table 2)
+They use (very) few classifiers. See table 4. I suspect this is as they want to use the genetic algorihtm after for 1000 rounds. Though, this beg the question what would happen if they had used more classifiers
+Ignores the longitudinal aspect of data by bagging all observations and only using one observation from each firm
+Skewed sampling with details omitted</t>
+  </si>
+  <si>
+    <t>Not clear whether the entire population of bankrupt firms is used. 50% control are seleceted though details are omitted</t>
+  </si>
+  <si>
+    <t>Cross validated AUC of at best 77%. Seems low given that you could get 75% in-sample by sorting by total assets</t>
+  </si>
+  <si>
+    <t>'1,200 externally audited manufacturing firms, half of which have gone bankrupt during
+2002–2005 while healthy firms have been selected from active companies at the end of 2005' from Korea</t>
+  </si>
+  <si>
+    <t>Examins the predictive perform through time with a model like Shumway 2001 for American listed firms
+Fits a simple 3 accoutning variable model acroos two different time periods and compares. Finds stable coeffecients and out-sample decile rankings 
+Easy to read
+Later they add marked values like Shumway (2001) expect that they use returns instead of excess returns
+I hesitate to say they conclusion of robustness could not just be a fact of the chosen periods 
+I dont get why they focus on the last three deciles in their deciles ranking. Failures outsite even the first decile should be of concern given the sparse amount of failures. See table table 5 panel E versus table 8 panel G. This comment is related to phrases like:' The overall predictive power of the combined model remains essentially unchanged when accuracy is measured with respect to the bottom three deciles'</t>
+  </si>
+  <si>
+    <t>Predict bankrupcty for Korean firms. Compares Neural Networks as is, with bagging and with AdaBoost. Finds improvments with both ensamble methods
+Results suggest that bagging might be slightly better
+AUCs seems low 
+Would be nice to know the details herof:' Several experiments were conducted to find the effects of the number of hidden nodes on the accuracy in predicting the test data set,'
+Would also be nice to know the details hereof:' Initially 32 financial ratios... are investigated ... Finally, 7 financial ratios with the highest accuracy ratio [AUC]'
+I figure they used the entire sample for the latter previous comment. I guess this could lead to overfitting issues. It seems that they used 10-fold cross validation for the former when you look at table 5
+I guess there is one record per firm 
+Bags all the results and ignores the temporal aspect of the data</t>
+  </si>
+  <si>
+    <t>How useful are auditors going concern opinions as predictors of default?</t>
+  </si>
+  <si>
+    <t>'2,770 firms, covering 392,404 firm-months of data' of which 175 defaults. See page 11 for further outcome definitions</t>
+  </si>
+  <si>
+    <t>US-listed industrial firms from 1980 to 2004
+Quaterly accounting data from Compustat with stock data from CRSP
+'... timing of default, merger, other-exit, and bankruptcy are mainly from Moodys Default Risk Service and the CRSP/Compustat database. For cases in which a firm exits our database and no exit reason appears in either of these sources, we refer to Bloomberg’s CACS function, SDC, CRSP, and, when necessary, other sources'
+Only firms with records in Compustat, CRSP and Moodys data base are included. Further only firm with Moodys ‘‘Industrial’’ category are included</t>
+  </si>
+  <si>
+    <t>Forecasts default for US listed firms. The instanous hazard is modelled by the exponential distribution with macro economic and firm specific covariates
+Firm specific covariates are modelled independently with a first-order Gaussian vector autoregressive model with mean reversion 
+Estimates merger and accusitions as a separate process
+The idea of modelling the covariate process is interesting. Whether the model they propose is suitable or not is not clear to me. Firstly, estimating target values for each firm as they do in (14) seems questionable for firms where we have little data. Further, I recall reading about other models for predicting accounting data which does fairly well. These could be used in place as the covariate process is assumed independent
+Their out-sample performance is quite high for one year ahead out-sample forecast. Though, their comparison Shumway (2001) and Beaver, McNichols, and Rhie (2005) on page 24 is questionable given that these papers work with a larger an possibly harder to clasify population</t>
+  </si>
+  <si>
+    <t>88% out-sample one year ahead accuracy ratio which they define as #the area between the power curve and the 45 line'
+This may explain why they later get negative estimates in table 3</t>
   </si>
 </sst>
 </file>
@@ -1634,13 +1774,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A64" sqref="A64"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1659,7 +1799,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -1674,7 +1814,7 @@
         <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="144" x14ac:dyDescent="0.3">
@@ -1729,7 +1869,7 @@
         <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="1">
         <v>5</v>
@@ -1749,7 +1889,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>21</v>
@@ -1758,7 +1898,7 @@
         <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="I4" s="1">
         <v>2</v>
@@ -1787,7 +1927,7 @@
         <v>34</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="1">
         <v>3</v>
@@ -1797,26 +1937,23 @@
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I6" s="1">
         <v>5</v>
@@ -1824,28 +1961,28 @@
     </row>
     <row r="7" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="I7" s="1">
         <v>2</v>
@@ -1853,28 +1990,28 @@
     </row>
     <row r="8" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I8" s="1">
         <v>1</v>
@@ -1882,28 +2019,25 @@
     </row>
     <row r="9" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="I9" s="1">
         <v>3</v>
@@ -1911,25 +2045,25 @@
     </row>
     <row r="10" spans="1:9" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="I10" s="1">
         <v>2</v>
@@ -1937,28 +2071,25 @@
     </row>
     <row r="11" spans="1:9" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="H11" s="1" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="I11" s="1">
         <v>3</v>
@@ -1966,25 +2097,25 @@
     </row>
     <row r="12" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I12" s="1">
         <v>5</v>
@@ -1992,22 +2123,22 @@
     </row>
     <row r="13" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I13" s="1">
         <v>5</v>
@@ -2015,22 +2146,22 @@
     </row>
     <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I14" s="1">
         <v>5</v>
@@ -2038,13 +2169,13 @@
     </row>
     <row r="15" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I15" s="1">
         <v>5</v>
@@ -2052,22 +2183,22 @@
     </row>
     <row r="16" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="I16" s="1">
         <v>5</v>
@@ -2075,25 +2206,25 @@
     </row>
     <row r="17" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="H17" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="I17" s="1">
         <v>3</v>
@@ -2101,25 +2232,25 @@
     </row>
     <row r="18" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="I18" s="1">
         <v>4</v>
@@ -2127,28 +2258,28 @@
     </row>
     <row r="19" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I19" s="1">
         <v>4</v>
@@ -2156,28 +2287,28 @@
     </row>
     <row r="20" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="I20" s="1">
         <v>4</v>
@@ -2185,25 +2316,25 @@
     </row>
     <row r="21" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="I21" s="1">
         <v>5</v>
@@ -2211,16 +2342,16 @@
     </row>
     <row r="22" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I22" s="1">
         <v>5</v>
@@ -2228,25 +2359,25 @@
     </row>
     <row r="23" spans="1:9" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="E23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="I23" s="1">
         <v>3</v>
@@ -2254,16 +2385,16 @@
     </row>
     <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I24" s="1">
         <v>5</v>
@@ -2271,28 +2402,28 @@
     </row>
     <row r="25" spans="1:9" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="H25" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="I25" s="1">
         <v>3</v>
@@ -2300,28 +2431,28 @@
     </row>
     <row r="26" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="I26" s="1">
         <v>3</v>
@@ -2329,28 +2460,28 @@
     </row>
     <row r="27" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I27" s="1">
         <v>4</v>
@@ -2358,25 +2489,25 @@
     </row>
     <row r="28" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="I28" s="1">
         <v>4</v>
@@ -2384,25 +2515,25 @@
     </row>
     <row r="29" spans="1:9" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>167</v>
       </c>
       <c r="I29" s="1">
         <v>1</v>
@@ -2410,7 +2541,7 @@
     </row>
     <row r="30" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>16</v>
@@ -2418,7 +2549,7 @@
     </row>
     <row r="31" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>29</v>
@@ -2426,7 +2557,7 @@
     </row>
     <row r="32" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>29</v>
@@ -2434,37 +2565,46 @@
     </row>
     <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I35" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>93</v>
+      <c r="G36" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>182</v>
@@ -2473,29 +2613,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="I37" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>188</v>
+      <c r="G38" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>189</v>
@@ -2504,137 +2653,140 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>190</v>
+      <c r="F39" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>193</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="I39" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I40" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="I40" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="I41" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="D42" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="H42" s="1" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="I42" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>215</v>
+      <c r="F43" s="2" t="s">
+        <v>221</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="I43" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="316.8" x14ac:dyDescent="0.3">
@@ -2645,413 +2797,562 @@
         <v>229</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="G44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="I44" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="316.8" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>73</v>
+      <c r="D45" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>231</v>
       </c>
       <c r="I45" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="I46" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>239</v>
-      </c>
       <c r="H47" s="1" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="I47" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>246</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F48" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>245</v>
       </c>
+      <c r="G48" s="1" t="s">
+        <v>247</v>
+      </c>
       <c r="H48" s="1" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="I48" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="374.4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>254</v>
+        <v>287</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>255</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>250</v>
-      </c>
       <c r="E49" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="I49" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>292</v>
+        <v>260</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>257</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>256</v>
+        <v>47</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I50" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H51" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="I51" s="1">
-        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="E53" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="H53" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="I53" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="I54" s="1">
-        <v>4</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>150</v>
+        <v>273</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I57" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="I58" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B59" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+      <c r="B60" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="I58" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="331.2" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    </row>
+    <row r="61" spans="1:9" ht="360" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D59" s="1" t="s">
+      <c r="C61" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="I61" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="I59" s="1">
+      <c r="H62" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="I62" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B61" s="1" t="s">
+    <row r="63" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+    <row r="64" spans="1:9" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="316.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="G63" s="1" t="s">
+      <c r="C64" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="I64" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="H63" s="1" t="s">
+      <c r="B65" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I63" s="1">
+      <c r="B66" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="I69" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="I70" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>314</v>
+    <row r="71" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="I73" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="345.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="I75" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new articles to read
</commit_message>
<xml_diff>
--- a/data/review_data.xlsx
+++ b/data/review_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="381">
   <si>
     <t>Article name</t>
   </si>
@@ -1411,6 +1411,106 @@
   <si>
     <t>88% out-sample one year ahead accuracy ratio which they define as #the area between the power curve and the 45 line'
 This may explain why they later get negative estimates in table 3</t>
+  </si>
+  <si>
+    <t>Bankruptcy prediction in banks and firms via statistical a intelligent techniques – a review</t>
+  </si>
+  <si>
+    <t>A comparative survey of artificial intelligence applications in finance artificial neural networks, expert systems and hybrid intelligent systems</t>
+  </si>
+  <si>
+    <t>Hybrid and ensemblebased soft computing techniques in bankruptcy prediction a survey</t>
+  </si>
+  <si>
+    <t>Machine learning in financial crisis prediction a survey</t>
+  </si>
+  <si>
+    <t>A quadratic interval logit model for forecasting bankruptcy</t>
+  </si>
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <t>Predicting the survival or failure of click-and-mortar corporations: A knowledge discovery approach</t>
+  </si>
+  <si>
+    <t>Forecasting financial condition of Chinese listed companies based on support vector machine</t>
+  </si>
+  <si>
+    <t>Predicting business failure using support vector machines with straightforward wrapper: A re-sampling study</t>
+  </si>
+  <si>
+    <t>From linear to non-linear kernel based classifiers for bankruptcy prediction</t>
+  </si>
+  <si>
+    <t>Neurocomputing</t>
+  </si>
+  <si>
+    <t>An Application of Support Vector Machine to Companies’ Financial Distress Prediction</t>
+  </si>
+  <si>
+    <t>A selective ensemble based on expected probabilities for bankruptcy prediction</t>
+  </si>
+  <si>
+    <t>Expert systems with applications</t>
+  </si>
+  <si>
+    <t>Integration of case-based forecasting, neural network, and discriminant analysis for bankruptcy prediction</t>
+  </si>
+  <si>
+    <t>Predicting business failure using classification and regression tree: An empirical comparison with popular classical statistical methods and top classification mining methods</t>
+  </si>
+  <si>
+    <t>The random subspace binary logit (RSBL) model for bankruptcy prediction</t>
+  </si>
+  <si>
+    <t>Principal component case-based reasoning ensemble for business failure prediction</t>
+  </si>
+  <si>
+    <t>Information &amp; Management</t>
+  </si>
+  <si>
+    <t>Firm bankruptcy prediction: experimental comparison of isotonic separation and other classification approaches</t>
+  </si>
+  <si>
+    <t>IEEE Transactions on Systems</t>
+  </si>
+  <si>
+    <t>A genetic algorithm application in bankruptcy prediction modeling</t>
+  </si>
+  <si>
+    <t>An application of support vector machines in bankruptcy prediction model</t>
+  </si>
+  <si>
+    <t>SFFS-PC-NN optimized by genetic algorithm for dynamic prediction of financial distress with longitudinal data streams</t>
+  </si>
+  <si>
+    <t>Listed companies’ financial distress prediction based on weighted majority voting combination of multiple classifiers</t>
+  </si>
+  <si>
+    <t>Dynamic financial distress prediction using instance selection for the disposal of concept drift</t>
+  </si>
+  <si>
+    <t>Feature selection in bankruptcy prediction</t>
+  </si>
+  <si>
+    <t>Concept Drift-Oriented Adaptive and Dynamic Support Vector Machine Ensemble With Time Window in Corporate Financial Risk Prediction</t>
+  </si>
+  <si>
+    <t>Review articles using "state-of-the-art" methods and catogrise them with respect to financial distress definition, methods, sampling and feature selection
+The methods section is intersting in that it covers more 'new-age' classifiers like SVM, NN, fuzzy-network, ensambles etc. The introduction to the various method is limited and more focus is put on the articles
+There were not any many insides for me in the sampling section and feature section. It may be useful if you searching for a reference to articles that samples as you do  
+Some of the comments are qustionable or out right wrong like:' However, it [logistic] still requires that the independent variables have no linear functional relationship with each other, namely, no multi-collinearity
+problem' (which is true if the are very linearly dependent of course but by no means require complete linear independence)</t>
+  </si>
+  <si>
+    <t>Using genetic algorithms to evolve type-2 fuzzy logic systems for predicting bankruptcy</t>
+  </si>
+  <si>
+    <t>Kybernetes</t>
+  </si>
+  <si>
+    <t>RE</t>
   </si>
 </sst>
 </file>
@@ -1774,13 +1874,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2797,7 +2897,7 @@
         <v>229</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>71</v>
+        <v>380</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>227</v>
@@ -3196,12 +3296,21 @@
         <v>306</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>307</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="I66" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -3349,6 +3458,185 @@
       </c>
       <c r="I75" s="1">
         <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated script to handle update of new and missing data
</commit_message>
<xml_diff>
--- a/data/review_data.xlsx
+++ b/data/review_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="405">
   <si>
     <t>Article name</t>
   </si>
@@ -1419,9 +1419,6 @@
     <t>A comparative survey of artificial intelligence applications in finance artificial neural networks, expert systems and hybrid intelligent systems</t>
   </si>
   <si>
-    <t>Hybrid and ensemblebased soft computing techniques in bankruptcy prediction a survey</t>
-  </si>
-  <si>
     <t>Machine learning in financial crisis prediction a survey</t>
   </si>
   <si>
@@ -1497,20 +1494,142 @@
     <t>Concept Drift-Oriented Adaptive and Dynamic Support Vector Machine Ensemble With Time Window in Corporate Financial Risk Prediction</t>
   </si>
   <si>
-    <t>Review articles using "state-of-the-art" methods and catogrise them with respect to financial distress definition, methods, sampling and feature selection
+    <t>Using genetic algorithms to evolve type-2 fuzzy logic systems for predicting bankruptcy</t>
+  </si>
+  <si>
+    <t>Kybernetes</t>
+  </si>
+  <si>
+    <t>'Matching method is utilized to choose normal
+non-financial-distress companies according to the following rules.
+(1) The matched two companies have the same or similar industry.
+(2) The chosen normal company should never be specially treated.
+(3) The matched two companies should have similar asset size in the range of [−30%, +30%]'</t>
+  </si>
+  <si>
+    <t>Chinese traded firms in 2000 to 2005
+Financial distress is defined as 'specially treated (ST) by Chinese Stock Exchange due to abnormal financial status'. That is two period of negative income or a further condition on the market to book ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">135 / 135 firms with what I guess is 1 set of accounting statements for each firm </t>
+  </si>
+  <si>
+    <t>82% accuracy out sample based on 30 times hold out experimints. The split is 2:1 strafied by distress or not. Though see the comment in my review about the ensamble training</t>
+  </si>
+  <si>
+    <t>Makes an ensamble of SVM with different feature spaces and different kernals functions
+Reduce the final ensamble with Q diversity meassure in a greedy process. The final predicition is based on weighted voting
+The feature selection seems questionable to me. While I do get why you would use PCA as you are going to use L2 norms later I do not see why you would use stepwise regression with multiple descrimination analysis or logistic regression to select features
+Feature selection is based on the entire population in hold-out test. See page 8 for details
+Use matched sampling
+This may not be a good pratice 'Sample companies with financial ratios deviating from the mean value as much as three times of standard deviation are excluded'
+If I get what they are saying on page 7 correclty ('candidate classifiers with relatively high cross validation accuracy on training dataset') then the ensamble is trained on the final testing data. If this is the case than it does not seem strange that the performance improves with the ensamble
+Cross-valdiation accuracy of 82% seems low given the above and what I have seen in other papers using matched samples for Chinese firms preidicting ST</t>
+  </si>
+  <si>
+    <t>US firms from 1970 to 2006
+Defaults from Moody’s Default Risk Service
+Firms issues are included if it '… is not a sovereign and has a senior rating'
+Their default definition seems broad to me (see page 6 under data). For example '51% of the defaults are due to missed interest payments'</t>
+  </si>
+  <si>
+    <t>SMR, CO, FR</t>
+  </si>
+  <si>
+    <t>Models aggreagate defaults count for US firms. The models includes both frailty and contagion. The intensity is a CIR process (which gives the frailty) with a term added for the counts of defaults (which gives the contagion). Different functions of the number of events is used for the contagion effect
+They use two macro economic variables in addition in the modelling (3 month Treasury bill yield and the trailing 1 year return on the S&amp;P 500 index). I guess a CIR process for the treasury bill and geomatric brownian motions for the S&amp;P returns is an ok choice for the models for these 
+I am not sure whether or not their test or estimation methods are a good idea. I would have to read up on counting process to evaluate this
+The two variables add little information to the model. Finds that the Hawkess process work rather well
+I would hesitate to conclude that this also applies for firms specefic models rather than default counting process. The paper may be interesting if you want to model aggregate counts. Though, I figure you might as well use a firm specific model with contagion an aggregate from this model
+Some notes that may be useful when reading: 
+- Zero-factor model: Hawkess process
+- One-factor model: CIR process with contagion effect
+- One-factor w/ covariates: replace the Brownian motion with one of the covariates</t>
+  </si>
+  <si>
+    <t>6048 firms in 2006
+1374 defaults through out the period</t>
+  </si>
+  <si>
+    <t>Integrating cognitive mapping and MCDA for bankruptcy prediction in small- and medium-sized enterprises</t>
+  </si>
+  <si>
+    <t>A Survival Approach to Prediction of Default Drivers for Indian Listed Companies</t>
+  </si>
+  <si>
+    <t>Hybrid and ensemble based soft computing techniques in bankruptcy prediction a survey</t>
+  </si>
+  <si>
+    <t>Review the following in default prediction using soft computing*: 
+ - Use dimension reduction methods
+ - What I would coin 'automatic' feature selection
+ - What they denote 'hybrid' method which is when more methods are used to model at the same time
+ - Ensamble methods with soft computing algorithms
+The article does not explain the methods but just who have used the different methods 
+The article may be useful a source for previous works with a given method
+The extend to which each methods is covered seems arbitrary to me
+The author states throughout that the results are not compared due to different data sets and validation methods. This is fair but some (subjective) opinion of the approach in the various papers would have been useful
+I do not find the notion of hybrid methods too useful. For instance, using a genetic alogrithm to select hyper-parameters and features in an SVM seems more like genreal optimization techince applied to SVM. Secondly, because the term does not seem convetional to me (though a google search do indicate that it is used) 
+* Soft computing: '... principal constituents of Soft Computing (SC) are Fuzzy Logic (FL), Evolutionary Computation (EC), Machine Learning (ML) and Probabilistic Reasoning (PR)' (source: wiki)</t>
+  </si>
+  <si>
+    <t>A survey of business failures with an emphasis on prediction methods and industrial applications</t>
+  </si>
+  <si>
+    <t>A semi-deterministic ensemble strategy for imbalanced datasets (SDEID) applied to bankruptcy prediction</t>
+  </si>
+  <si>
+    <t>Variable selection in high-dimensional regression: a nonparametric procedure for business failure prediction</t>
+  </si>
+  <si>
+    <t>An out-of-sample evaluation framework for DEA with application in bankruptcy prediction</t>
+  </si>
+  <si>
+    <t>Financial distress prediction: The case of French small and medium-sized firms</t>
+  </si>
+  <si>
+    <t>Bankruptcy prediction in banks by fuzzy rulebased classifier</t>
+  </si>
+  <si>
+    <t>Review articles using 'state-of-the-art' methods and catogrise them with respect to financial distress definition, methods, sampling and feature selection
 The methods section is intersting in that it covers more 'new-age' classifiers like SVM, NN, fuzzy-network, ensambles etc. The introduction to the various method is limited and more focus is put on the articles
 There were not any many insides for me in the sampling section and feature section. It may be useful if you searching for a reference to articles that samples as you do  
 Some of the comments are qustionable or out right wrong like:' However, it [logistic] still requires that the independent variables have no linear functional relationship with each other, namely, no multi-collinearity
 problem' (which is true if the are very linearly dependent of course but by no means require complete linear independence)</t>
   </si>
   <si>
-    <t>Using genetic algorithms to evolve type-2 fuzzy logic systems for predicting bankruptcy</t>
-  </si>
-  <si>
-    <t>Kybernetes</t>
-  </si>
-  <si>
-    <t>RE</t>
+    <t>587 / 3183 firms with  22231 nonbankruptcy firm-years</t>
+  </si>
+  <si>
+    <t>From what I gather, the non-bankrupt firms are sampled. I figure so from this comment:' Nonbankrupt firms with complete information randomly selected in the periods of 1991–2002'</t>
+  </si>
+  <si>
+    <t>Bootstraps Estimated Misclassification Cost (EMC) for a grid of different relative costs</t>
+  </si>
+  <si>
+    <t>US-listed firms on NASDAQ, AMEX and NYSE from 1991 to 2001
+Defaults are from Compustat and Lexis-Nexis Bankruptcy Report databases
+Financial data from Compustat and 'Auditors’ going concern opinions are obtained by anually reading auditors’ reports' 
+Firms are excluded from the financial industry group (SIC 6000–6999) or utility (SIC 4900–4999) industries
+Firms are excluded who do not have a 10-K and 20-k filed prior (as far as I gather though they later write that only collect these for the test sample so I am not sure how this is done)</t>
+  </si>
+  <si>
+    <t>Fits a hazard model like Shumway (2001)
+It seems like a lot observations are excluded who does not have a 10-K filed prior
+I don’t see why they exclude the utility firms and sample the non-bankerupt firms. The articles is from 2006 so estimating the logit a model for the full sample should be durable
+I guess including Current Assets/Total Assets and Cash/Total Assets could lead to multicollinearity issues
+Uses lagged year default rates based on two digits SIC codes. May be a good idea though I figure som of the two digits SIC codes groups will be sparse. The issues with the two digits level is further stressed in this later comment:' The average annual industry failure rate is 1.35%. Note that some high industry failure rates are driven by the small number of firms existing in the industry' 
+Uses cutoffs and Estimated Misclassification Cost (EMC) which I am not a fan of due to the arbitrariness of the relative cost and cutoff level
+I do not get why they add 'the composite stress measure' instead of just including the terms. E.g. for Zmijewski probability which consists of a lot of variables they already include and an rather arbitrary cutoff of 28% 
+I do not get this comment when they bootstrap the EMC:' There is no need to randomly select bankrupt firms since they are deterministic'
+I will need to read up on the bootsrap procedure on page 73. The results suggest that the hazard models does better than the auditors opinions for most cost levels
+The binary for the auditors opinon has an increase in odds of exp(1.8) when added to the model</t>
+  </si>
+  <si>
+    <t>RA, LDA, NN, B, BA, SVM, AdaBoost, CL, LOGI, GAM, SMR</t>
+  </si>
+  <si>
+    <t>Risk Management</t>
   </si>
 </sst>
 </file>
@@ -1874,13 +1993,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomRight" activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2166,7 +2285,7 @@
         <v>65</v>
       </c>
       <c r="I10" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="403.2" x14ac:dyDescent="0.3">
@@ -2897,7 +3016,7 @@
         <v>229</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>380</v>
+        <v>353</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>227</v>
@@ -3106,12 +3225,30 @@
         <v>147</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>272</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>273</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="I55" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -3188,12 +3325,33 @@
         <v>147</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>278</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>279</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="I60" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="360" x14ac:dyDescent="0.3">
@@ -3288,191 +3446,197 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="I65" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="I66" s="1">
-        <v>4</v>
+        <v>309</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="C68" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="I68" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B69" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="I69" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="I69" s="1">
+      <c r="C72" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="I72" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="345.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="I74" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="I70" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="I73" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="I75" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>351</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="I78" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -3480,17 +3644,20 @@
         <v>352</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B81" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>356</v>
       </c>
@@ -3498,19 +3665,16 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>357</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>29</v>
+        <v>358</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="B84" s="1" t="s">
         <v>359</v>
       </c>
     </row>
@@ -3518,16 +3682,19 @@
       <c r="A85" s="1" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B85" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>363</v>
       </c>
@@ -3535,12 +3702,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>364</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -3548,23 +3715,23 @@
         <v>365</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>369</v>
+        <v>29</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -3575,12 +3742,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>371</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -3588,7 +3755,7 @@
         <v>372</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -3599,7 +3766,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>374</v>
       </c>
@@ -3607,36 +3774,86 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="I97" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
-        <v>305</v>
-      </c>
       <c r="B98" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>376</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>379</v>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>